<commit_message>
eCRF journal export permissions
</commit_message>
<xml_diff>
--- a/permission_definitions.xlsx
+++ b/permission_definitions.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7588" uniqueCount="1905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7593" uniqueCount="1906">
   <si>
     <t>INVENTORY_DB</t>
   </si>
@@ -5741,6 +5741,9 @@
   </si>
   <si>
     <t>TRIAL_SIGNUP</t>
+  </si>
+  <si>
+    <t>org.phoenixctms.ctsms.service.shared.JournalService.exportEcrfJournal</t>
   </si>
 </sst>
 </file>
@@ -8812,10 +8815,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I1276"/>
+  <dimension ref="A2:I1278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A868" workbookViewId="0">
-      <selection activeCell="A905" sqref="A905"/>
+    <sheetView tabSelected="1" topLeftCell="A1076" workbookViewId="0">
+      <selection activeCell="A1091" sqref="A1091"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -25430,42 +25433,19 @@
     </row>
     <row r="1092" spans="1:9">
       <c r="A1092" t="s">
-        <v>1666</v>
+        <v>1905</v>
+      </c>
+      <c r="B1092" t="s">
+        <v>1192</v>
       </c>
       <c r="C1092" t="s">
-        <v>740</v>
-      </c>
-      <c r="D1092" t="s">
-        <v>741</v>
+        <v>228</v>
       </c>
       <c r="E1092" t="s">
-        <v>710</v>
-      </c>
-      <c r="F1092" t="s">
-        <v>1667</v>
+        <v>720</v>
       </c>
       <c r="I1092" t="s">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="1093" spans="1:9">
-      <c r="A1093" t="s">
-        <v>1666</v>
-      </c>
-      <c r="C1093" t="s">
-        <v>740</v>
-      </c>
-      <c r="D1093" t="s">
-        <v>742</v>
-      </c>
-      <c r="E1093" t="s">
-        <v>718</v>
-      </c>
-      <c r="F1093" t="s">
-        <v>1667</v>
-      </c>
-      <c r="I1093" s="1" t="s">
-        <v>1071</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="1094" spans="1:9">
@@ -25476,102 +25456,102 @@
         <v>740</v>
       </c>
       <c r="D1094" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="E1094" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="F1094" t="s">
         <v>1667</v>
       </c>
       <c r="I1094" t="s">
-        <v>1104</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="1095" spans="1:9">
       <c r="A1095" t="s">
         <v>1666</v>
       </c>
-      <c r="B1095" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1095" t="s">
         <v>740</v>
       </c>
       <c r="D1095" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="E1095" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="F1095" t="s">
         <v>1667</v>
       </c>
-      <c r="I1095" t="s">
-        <v>1077</v>
+      <c r="I1095" s="1" t="s">
+        <v>1071</v>
       </c>
     </row>
     <row r="1096" spans="1:9">
       <c r="A1096" t="s">
         <v>1666</v>
       </c>
-      <c r="B1096" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1096" t="s">
         <v>740</v>
       </c>
       <c r="D1096" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="E1096" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="F1096" t="s">
         <v>1667</v>
       </c>
       <c r="I1096" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="1097" spans="1:9">
       <c r="A1097" t="s">
         <v>1666</v>
       </c>
+      <c r="B1097" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1097" t="s">
         <v>740</v>
       </c>
       <c r="D1097" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E1097" t="s">
-        <v>748</v>
+        <v>720</v>
       </c>
       <c r="F1097" t="s">
         <v>1667</v>
       </c>
       <c r="I1097" t="s">
-        <v>1108</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="1098" spans="1:9">
       <c r="A1098" t="s">
         <v>1666</v>
       </c>
+      <c r="B1098" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1098" t="s">
         <v>740</v>
       </c>
       <c r="D1098" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="E1098" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="F1098" t="s">
         <v>1667</v>
       </c>
       <c r="I1098" t="s">
-        <v>1113</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="1099" spans="1:9">
@@ -25582,16 +25562,16 @@
         <v>740</v>
       </c>
       <c r="D1099" t="s">
-        <v>783</v>
+        <v>746</v>
       </c>
       <c r="E1099" t="s">
-        <v>658</v>
+        <v>748</v>
       </c>
       <c r="F1099" t="s">
         <v>1667</v>
       </c>
       <c r="I1099" t="s">
-        <v>1120</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="1100" spans="1:9">
@@ -25602,16 +25582,16 @@
         <v>740</v>
       </c>
       <c r="D1100" t="s">
-        <v>783</v>
+        <v>747</v>
       </c>
       <c r="E1100" t="s">
-        <v>661</v>
+        <v>722</v>
       </c>
       <c r="F1100" t="s">
         <v>1667</v>
       </c>
       <c r="I1100" t="s">
-        <v>1127</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="1101" spans="1:9">
@@ -25625,13 +25605,13 @@
         <v>783</v>
       </c>
       <c r="E1101" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F1101" t="s">
         <v>1667</v>
       </c>
       <c r="I1101" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1102" spans="1:9">
@@ -25645,22 +25625,19 @@
         <v>783</v>
       </c>
       <c r="E1102" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F1102" t="s">
         <v>1667</v>
       </c>
       <c r="I1102" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1103" spans="1:9">
       <c r="A1103" t="s">
         <v>1666</v>
       </c>
-      <c r="B1103" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1103" t="s">
         <v>740</v>
       </c>
@@ -25668,13 +25645,13 @@
         <v>783</v>
       </c>
       <c r="E1103" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F1103" t="s">
         <v>1667</v>
       </c>
       <c r="I1103" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1104" spans="1:9">
@@ -25688,19 +25665,22 @@
         <v>783</v>
       </c>
       <c r="E1104" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F1104" t="s">
         <v>1667</v>
       </c>
       <c r="I1104" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1105" spans="1:9">
       <c r="A1105" t="s">
         <v>1666</v>
       </c>
+      <c r="B1105" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1105" t="s">
         <v>740</v>
       </c>
@@ -25708,35 +25688,58 @@
         <v>783</v>
       </c>
       <c r="E1105" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F1105" t="s">
         <v>1667</v>
       </c>
       <c r="I1105" t="s">
-        <v>1132</v>
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:9">
+      <c r="A1106" t="s">
+        <v>1666</v>
+      </c>
+      <c r="C1106" t="s">
+        <v>740</v>
+      </c>
+      <c r="D1106" t="s">
+        <v>783</v>
+      </c>
+      <c r="E1106" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1106" t="s">
+        <v>1667</v>
+      </c>
+      <c r="I1106" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="1107" spans="1:9">
       <c r="A1107" t="s">
-        <v>1668</v>
-      </c>
-      <c r="B1107" t="s">
-        <v>1192</v>
+        <v>1666</v>
       </c>
       <c r="C1107" t="s">
-        <v>703</v>
+        <v>740</v>
+      </c>
+      <c r="D1107" t="s">
+        <v>783</v>
       </c>
       <c r="E1107" t="s">
-        <v>749</v>
+        <v>666</v>
+      </c>
+      <c r="F1107" t="s">
+        <v>1667</v>
       </c>
       <c r="I1107" t="s">
-        <v>1109</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1109" spans="1:9">
       <c r="A1109" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="B1109" t="s">
         <v>1192</v>
@@ -25748,47 +25751,24 @@
         <v>749</v>
       </c>
       <c r="I1109" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="1111" spans="1:9">
       <c r="A1111" t="s">
-        <v>1670</v>
+        <v>1669</v>
+      </c>
+      <c r="B1111" t="s">
+        <v>1192</v>
       </c>
       <c r="C1111" t="s">
-        <v>600</v>
-      </c>
-      <c r="D1111" t="s">
-        <v>1167</v>
+        <v>703</v>
       </c>
       <c r="E1111" t="s">
-        <v>658</v>
-      </c>
-      <c r="F1111" t="s">
-        <v>1671</v>
+        <v>749</v>
       </c>
       <c r="I1111" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="1112" spans="1:9">
-      <c r="A1112" t="s">
-        <v>1670</v>
-      </c>
-      <c r="C1112" t="s">
-        <v>600</v>
-      </c>
-      <c r="D1112" t="s">
-        <v>1167</v>
-      </c>
-      <c r="E1112" t="s">
-        <v>661</v>
-      </c>
-      <c r="F1112" t="s">
-        <v>1671</v>
-      </c>
-      <c r="I1112" t="s">
-        <v>1127</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="1113" spans="1:9">
@@ -25802,13 +25782,13 @@
         <v>1167</v>
       </c>
       <c r="E1113" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F1113" t="s">
         <v>1671</v>
       </c>
       <c r="I1113" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1114" spans="1:9">
@@ -25822,22 +25802,19 @@
         <v>1167</v>
       </c>
       <c r="E1114" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F1114" t="s">
         <v>1671</v>
       </c>
       <c r="I1114" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1115" spans="1:9">
       <c r="A1115" t="s">
         <v>1670</v>
       </c>
-      <c r="B1115" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1115" t="s">
         <v>600</v>
       </c>
@@ -25845,13 +25822,13 @@
         <v>1167</v>
       </c>
       <c r="E1115" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F1115" t="s">
         <v>1671</v>
       </c>
       <c r="I1115" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1116" spans="1:9">
@@ -25865,19 +25842,22 @@
         <v>1167</v>
       </c>
       <c r="E1116" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F1116" t="s">
         <v>1671</v>
       </c>
       <c r="I1116" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1117" spans="1:9">
       <c r="A1117" t="s">
         <v>1670</v>
       </c>
+      <c r="B1117" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1117" t="s">
         <v>600</v>
       </c>
@@ -25885,47 +25865,53 @@
         <v>1167</v>
       </c>
       <c r="E1117" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F1117" t="s">
         <v>1671</v>
       </c>
       <c r="I1117" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:9">
+      <c r="A1118" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C1118" t="s">
+        <v>600</v>
+      </c>
+      <c r="D1118" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E1118" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1118" t="s">
+        <v>1671</v>
+      </c>
+      <c r="I1118" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:9">
+      <c r="A1119" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C1119" t="s">
+        <v>600</v>
+      </c>
+      <c r="D1119" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E1119" t="s">
+        <v>666</v>
+      </c>
+      <c r="F1119" t="s">
+        <v>1671</v>
+      </c>
+      <c r="I1119" t="s">
         <v>1132</v>
-      </c>
-    </row>
-    <row r="1132" spans="1:9">
-      <c r="A1132" t="s">
-        <v>1672</v>
-      </c>
-      <c r="C1132" t="s">
-        <v>657</v>
-      </c>
-      <c r="E1132" t="s">
-        <v>658</v>
-      </c>
-      <c r="F1132" t="s">
-        <v>1673</v>
-      </c>
-      <c r="I1132" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="1133" spans="1:9">
-      <c r="A1133" t="s">
-        <v>1672</v>
-      </c>
-      <c r="C1133" t="s">
-        <v>657</v>
-      </c>
-      <c r="E1133" t="s">
-        <v>661</v>
-      </c>
-      <c r="F1133" t="s">
-        <v>1673</v>
-      </c>
-      <c r="I1133" t="s">
-        <v>1121</v>
       </c>
     </row>
     <row r="1134" spans="1:9">
@@ -25936,13 +25922,13 @@
         <v>657</v>
       </c>
       <c r="E1134" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F1134" t="s">
         <v>1673</v>
       </c>
       <c r="I1134" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="1135" spans="1:9">
@@ -25953,33 +25939,30 @@
         <v>657</v>
       </c>
       <c r="E1135" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F1135" t="s">
         <v>1673</v>
       </c>
       <c r="I1135" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="1136" spans="1:9">
       <c r="A1136" t="s">
         <v>1672</v>
       </c>
-      <c r="B1136" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1136" t="s">
         <v>657</v>
       </c>
       <c r="E1136" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F1136" t="s">
         <v>1673</v>
       </c>
       <c r="I1136" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="1137" spans="1:9">
@@ -25990,67 +25973,67 @@
         <v>657</v>
       </c>
       <c r="E1137" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F1137" t="s">
         <v>1673</v>
       </c>
       <c r="I1137" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="1138" spans="1:9">
       <c r="A1138" t="s">
         <v>1672</v>
       </c>
+      <c r="B1138" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1138" t="s">
         <v>657</v>
       </c>
       <c r="E1138" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F1138" t="s">
         <v>1673</v>
       </c>
       <c r="I1138" t="s">
-        <v>1126</v>
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:9">
+      <c r="A1139" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1139" t="s">
+        <v>657</v>
+      </c>
+      <c r="E1139" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1139" t="s">
+        <v>1673</v>
+      </c>
+      <c r="I1139" t="s">
+        <v>1125</v>
       </c>
     </row>
     <row r="1140" spans="1:9">
       <c r="A1140" t="s">
-        <v>1674</v>
+        <v>1672</v>
       </c>
       <c r="C1140" t="s">
-        <v>1153</v>
-      </c>
-      <c r="D1140" t="s">
-        <v>670</v>
+        <v>657</v>
       </c>
       <c r="E1140" t="s">
-        <v>658</v>
+        <v>666</v>
       </c>
       <c r="F1140" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
       <c r="I1140" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="1141" spans="1:9">
-      <c r="A1141" t="s">
-        <v>1674</v>
-      </c>
-      <c r="C1141" t="s">
-        <v>671</v>
-      </c>
-      <c r="E1141" t="s">
-        <v>658</v>
-      </c>
-      <c r="F1141" t="s">
-        <v>1676</v>
-      </c>
-      <c r="I1141" t="s">
-        <v>1119</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="1142" spans="1:9">
@@ -26064,13 +26047,13 @@
         <v>670</v>
       </c>
       <c r="E1142" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="F1142" t="s">
         <v>1675</v>
       </c>
       <c r="I1142" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="1143" spans="1:9">
@@ -26081,13 +26064,13 @@
         <v>671</v>
       </c>
       <c r="E1143" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="F1143" t="s">
         <v>1676</v>
       </c>
       <c r="I1143" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="1144" spans="1:9">
@@ -26101,13 +26084,13 @@
         <v>670</v>
       </c>
       <c r="E1144" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F1144" t="s">
         <v>1675</v>
       </c>
       <c r="I1144" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="1145" spans="1:9">
@@ -26118,13 +26101,13 @@
         <v>671</v>
       </c>
       <c r="E1145" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F1145" t="s">
         <v>1676</v>
       </c>
       <c r="I1145" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="1146" spans="1:9">
@@ -26138,13 +26121,13 @@
         <v>670</v>
       </c>
       <c r="E1146" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F1146" t="s">
         <v>1675</v>
       </c>
       <c r="I1146" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="1147" spans="1:9">
@@ -26155,22 +26138,19 @@
         <v>671</v>
       </c>
       <c r="E1147" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F1147" t="s">
         <v>1676</v>
       </c>
       <c r="I1147" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="1148" spans="1:9">
       <c r="A1148" t="s">
         <v>1674</v>
       </c>
-      <c r="B1148" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1148" t="s">
         <v>1153</v>
       </c>
@@ -26178,13 +26158,13 @@
         <v>670</v>
       </c>
       <c r="E1148" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F1148" t="s">
         <v>1675</v>
       </c>
       <c r="I1148" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="1149" spans="1:9">
@@ -26195,19 +26175,22 @@
         <v>671</v>
       </c>
       <c r="E1149" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F1149" t="s">
         <v>1676</v>
       </c>
       <c r="I1149" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="1150" spans="1:9">
       <c r="A1150" t="s">
         <v>1674</v>
       </c>
+      <c r="B1150" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1150" t="s">
         <v>1153</v>
       </c>
@@ -26215,13 +26198,13 @@
         <v>670</v>
       </c>
       <c r="E1150" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F1150" t="s">
         <v>1675</v>
       </c>
       <c r="I1150" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="1151" spans="1:9">
@@ -26232,13 +26215,13 @@
         <v>671</v>
       </c>
       <c r="E1151" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F1151" t="s">
         <v>1676</v>
       </c>
       <c r="I1151" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="1152" spans="1:9">
@@ -26252,13 +26235,13 @@
         <v>670</v>
       </c>
       <c r="E1152" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F1152" t="s">
         <v>1675</v>
       </c>
       <c r="I1152" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="1153" spans="1:9">
@@ -26269,53 +26252,50 @@
         <v>671</v>
       </c>
       <c r="E1153" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F1153" t="s">
         <v>1676</v>
       </c>
       <c r="I1153" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:9">
+      <c r="A1154" t="s">
+        <v>1674</v>
+      </c>
+      <c r="C1154" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D1154" t="s">
+        <v>670</v>
+      </c>
+      <c r="E1154" t="s">
+        <v>666</v>
+      </c>
+      <c r="F1154" t="s">
+        <v>1675</v>
+      </c>
+      <c r="I1154" t="s">
         <v>1126</v>
       </c>
     </row>
     <row r="1155" spans="1:9">
       <c r="A1155" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="C1155" t="s">
-        <v>585</v>
-      </c>
-      <c r="D1155" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="E1155" t="s">
-        <v>658</v>
+        <v>666</v>
       </c>
       <c r="F1155" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
       <c r="I1155" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="1156" spans="1:9">
-      <c r="A1156" t="s">
-        <v>1677</v>
-      </c>
-      <c r="C1156" t="s">
-        <v>585</v>
-      </c>
-      <c r="D1156" t="s">
-        <v>670</v>
-      </c>
-      <c r="E1156" t="s">
-        <v>661</v>
-      </c>
-      <c r="F1156" t="s">
-        <v>1678</v>
-      </c>
-      <c r="I1156" t="s">
-        <v>1121</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="1157" spans="1:9">
@@ -26329,13 +26309,13 @@
         <v>670</v>
       </c>
       <c r="E1157" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F1157" t="s">
         <v>1678</v>
       </c>
       <c r="I1157" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="1158" spans="1:9">
@@ -26349,22 +26329,19 @@
         <v>670</v>
       </c>
       <c r="E1158" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F1158" t="s">
         <v>1678</v>
       </c>
       <c r="I1158" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="1159" spans="1:9">
       <c r="A1159" t="s">
         <v>1677</v>
       </c>
-      <c r="B1159" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1159" t="s">
         <v>585</v>
       </c>
@@ -26372,13 +26349,13 @@
         <v>670</v>
       </c>
       <c r="E1159" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F1159" t="s">
         <v>1678</v>
       </c>
       <c r="I1159" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="1160" spans="1:9">
@@ -26392,19 +26369,22 @@
         <v>670</v>
       </c>
       <c r="E1160" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F1160" t="s">
         <v>1678</v>
       </c>
       <c r="I1160" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="1161" spans="1:9">
       <c r="A1161" t="s">
         <v>1677</v>
       </c>
+      <c r="B1161" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1161" t="s">
         <v>585</v>
       </c>
@@ -26412,18 +26392,38 @@
         <v>670</v>
       </c>
       <c r="E1161" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F1161" t="s">
         <v>1678</v>
       </c>
       <c r="I1161" t="s">
-        <v>1126</v>
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:9">
+      <c r="A1162" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C1162" t="s">
+        <v>585</v>
+      </c>
+      <c r="D1162" t="s">
+        <v>670</v>
+      </c>
+      <c r="E1162" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1162" t="s">
+        <v>1678</v>
+      </c>
+      <c r="I1162" t="s">
+        <v>1125</v>
       </c>
     </row>
     <row r="1163" spans="1:9">
       <c r="A1163" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="C1163" t="s">
         <v>585</v>
@@ -26432,33 +26432,13 @@
         <v>670</v>
       </c>
       <c r="E1163" t="s">
-        <v>658</v>
+        <v>666</v>
       </c>
       <c r="F1163" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
       <c r="I1163" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="1164" spans="1:9">
-      <c r="A1164" t="s">
-        <v>1679</v>
-      </c>
-      <c r="C1164" t="s">
-        <v>585</v>
-      </c>
-      <c r="D1164" t="s">
-        <v>670</v>
-      </c>
-      <c r="E1164" t="s">
-        <v>661</v>
-      </c>
-      <c r="F1164" t="s">
-        <v>1680</v>
-      </c>
-      <c r="I1164" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="1165" spans="1:9">
@@ -26472,13 +26452,13 @@
         <v>670</v>
       </c>
       <c r="E1165" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F1165" t="s">
         <v>1680</v>
       </c>
       <c r="I1165" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1166" spans="1:9">
@@ -26492,22 +26472,19 @@
         <v>670</v>
       </c>
       <c r="E1166" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F1166" t="s">
         <v>1680</v>
       </c>
       <c r="I1166" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1167" spans="1:9">
       <c r="A1167" t="s">
         <v>1679</v>
       </c>
-      <c r="B1167" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1167" t="s">
         <v>585</v>
       </c>
@@ -26515,13 +26492,13 @@
         <v>670</v>
       </c>
       <c r="E1167" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F1167" t="s">
         <v>1680</v>
       </c>
       <c r="I1167" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1168" spans="1:9">
@@ -26535,19 +26512,22 @@
         <v>670</v>
       </c>
       <c r="E1168" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F1168" t="s">
         <v>1680</v>
       </c>
       <c r="I1168" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1169" spans="1:9">
       <c r="A1169" t="s">
         <v>1679</v>
       </c>
+      <c r="B1169" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1169" t="s">
         <v>585</v>
       </c>
@@ -26555,47 +26535,53 @@
         <v>670</v>
       </c>
       <c r="E1169" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F1169" t="s">
         <v>1680</v>
       </c>
       <c r="I1169" t="s">
-        <v>1132</v>
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:9">
+      <c r="A1170" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C1170" t="s">
+        <v>585</v>
+      </c>
+      <c r="D1170" t="s">
+        <v>670</v>
+      </c>
+      <c r="E1170" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1170" t="s">
+        <v>1680</v>
+      </c>
+      <c r="I1170" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="1171" spans="1:9">
       <c r="A1171" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="C1171" t="s">
-        <v>600</v>
+        <v>585</v>
+      </c>
+      <c r="D1171" t="s">
+        <v>670</v>
       </c>
       <c r="E1171" t="s">
-        <v>658</v>
+        <v>666</v>
       </c>
       <c r="F1171" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
       <c r="I1171" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="1172" spans="1:9">
-      <c r="A1172" t="s">
-        <v>1681</v>
-      </c>
-      <c r="C1172" t="s">
-        <v>600</v>
-      </c>
-      <c r="E1172" t="s">
-        <v>661</v>
-      </c>
-      <c r="F1172" t="s">
-        <v>1682</v>
-      </c>
-      <c r="I1172" t="s">
-        <v>1127</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1173" spans="1:9">
@@ -26606,13 +26592,13 @@
         <v>600</v>
       </c>
       <c r="E1173" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F1173" t="s">
         <v>1682</v>
       </c>
       <c r="I1173" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1174" spans="1:9">
@@ -26623,33 +26609,30 @@
         <v>600</v>
       </c>
       <c r="E1174" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F1174" t="s">
         <v>1682</v>
       </c>
       <c r="I1174" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1175" spans="1:9">
       <c r="A1175" t="s">
         <v>1681</v>
       </c>
-      <c r="B1175" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1175" t="s">
         <v>600</v>
       </c>
       <c r="E1175" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F1175" t="s">
         <v>1682</v>
       </c>
       <c r="I1175" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1176" spans="1:9">
@@ -26660,64 +26643,67 @@
         <v>600</v>
       </c>
       <c r="E1176" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F1176" t="s">
         <v>1682</v>
       </c>
       <c r="I1176" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1177" spans="1:9">
       <c r="A1177" t="s">
         <v>1681</v>
       </c>
+      <c r="B1177" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1177" t="s">
         <v>600</v>
       </c>
       <c r="E1177" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F1177" t="s">
         <v>1682</v>
       </c>
       <c r="I1177" t="s">
-        <v>1132</v>
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:9">
+      <c r="A1178" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C1178" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1178" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1178" t="s">
+        <v>1682</v>
+      </c>
+      <c r="I1178" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="1179" spans="1:9">
       <c r="A1179" t="s">
-        <v>1836</v>
+        <v>1681</v>
       </c>
       <c r="C1179" t="s">
         <v>600</v>
       </c>
       <c r="E1179" t="s">
-        <v>658</v>
+        <v>666</v>
       </c>
       <c r="F1179" t="s">
-        <v>1837</v>
+        <v>1682</v>
       </c>
       <c r="I1179" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="1180" spans="1:9">
-      <c r="A1180" t="s">
-        <v>1836</v>
-      </c>
-      <c r="C1180" t="s">
-        <v>600</v>
-      </c>
-      <c r="E1180" t="s">
-        <v>661</v>
-      </c>
-      <c r="F1180" t="s">
-        <v>1837</v>
-      </c>
-      <c r="I1180" t="s">
-        <v>1127</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1181" spans="1:9">
@@ -26728,13 +26714,13 @@
         <v>600</v>
       </c>
       <c r="E1181" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F1181" t="s">
         <v>1837</v>
       </c>
       <c r="I1181" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1182" spans="1:9">
@@ -26745,33 +26731,30 @@
         <v>600</v>
       </c>
       <c r="E1182" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F1182" t="s">
         <v>1837</v>
       </c>
       <c r="I1182" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1183" spans="1:9">
       <c r="A1183" t="s">
         <v>1836</v>
       </c>
-      <c r="B1183" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1183" t="s">
         <v>600</v>
       </c>
       <c r="E1183" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F1183" t="s">
         <v>1837</v>
       </c>
       <c r="I1183" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1184" spans="1:9">
@@ -26782,70 +26765,67 @@
         <v>600</v>
       </c>
       <c r="E1184" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F1184" t="s">
         <v>1837</v>
       </c>
       <c r="I1184" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1185" spans="1:9">
       <c r="A1185" t="s">
         <v>1836</v>
       </c>
+      <c r="B1185" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1185" t="s">
         <v>600</v>
       </c>
       <c r="E1185" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F1185" t="s">
         <v>1837</v>
       </c>
       <c r="I1185" t="s">
-        <v>1132</v>
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:9">
+      <c r="A1186" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C1186" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1186" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1186" t="s">
+        <v>1837</v>
+      </c>
+      <c r="I1186" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="1187" spans="1:9">
       <c r="A1187" t="s">
-        <v>1838</v>
+        <v>1836</v>
       </c>
       <c r="C1187" t="s">
-        <v>585</v>
-      </c>
-      <c r="D1187" t="s">
-        <v>670</v>
+        <v>600</v>
       </c>
       <c r="E1187" t="s">
-        <v>658</v>
+        <v>666</v>
       </c>
       <c r="F1187" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="I1187" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="1188" spans="1:9">
-      <c r="A1188" t="s">
-        <v>1838</v>
-      </c>
-      <c r="C1188" t="s">
-        <v>585</v>
-      </c>
-      <c r="D1188" t="s">
-        <v>670</v>
-      </c>
-      <c r="E1188" t="s">
-        <v>661</v>
-      </c>
-      <c r="F1188" t="s">
-        <v>1839</v>
-      </c>
-      <c r="I1188" t="s">
-        <v>1127</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1189" spans="1:9">
@@ -26859,13 +26839,13 @@
         <v>670</v>
       </c>
       <c r="E1189" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F1189" t="s">
         <v>1839</v>
       </c>
       <c r="I1189" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1190" spans="1:9">
@@ -26879,22 +26859,19 @@
         <v>670</v>
       </c>
       <c r="E1190" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F1190" t="s">
         <v>1839</v>
       </c>
       <c r="I1190" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1191" spans="1:9">
       <c r="A1191" t="s">
         <v>1838</v>
       </c>
-      <c r="B1191" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1191" t="s">
         <v>585</v>
       </c>
@@ -26902,13 +26879,13 @@
         <v>670</v>
       </c>
       <c r="E1191" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F1191" t="s">
         <v>1839</v>
       </c>
       <c r="I1191" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1192" spans="1:9">
@@ -26922,19 +26899,22 @@
         <v>670</v>
       </c>
       <c r="E1192" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F1192" t="s">
         <v>1839</v>
       </c>
       <c r="I1192" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1193" spans="1:9">
       <c r="A1193" t="s">
         <v>1838</v>
       </c>
+      <c r="B1193" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1193" t="s">
         <v>585</v>
       </c>
@@ -26942,47 +26922,53 @@
         <v>670</v>
       </c>
       <c r="E1193" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F1193" t="s">
         <v>1839</v>
       </c>
       <c r="I1193" t="s">
-        <v>1132</v>
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:9">
+      <c r="A1194" t="s">
+        <v>1838</v>
+      </c>
+      <c r="C1194" t="s">
+        <v>585</v>
+      </c>
+      <c r="D1194" t="s">
+        <v>670</v>
+      </c>
+      <c r="E1194" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1194" t="s">
+        <v>1839</v>
+      </c>
+      <c r="I1194" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="1195" spans="1:9">
       <c r="A1195" t="s">
-        <v>1683</v>
+        <v>1838</v>
       </c>
       <c r="C1195" t="s">
-        <v>600</v>
+        <v>585</v>
+      </c>
+      <c r="D1195" t="s">
+        <v>670</v>
       </c>
       <c r="E1195" t="s">
-        <v>658</v>
+        <v>666</v>
       </c>
       <c r="F1195" t="s">
-        <v>1684</v>
+        <v>1839</v>
       </c>
       <c r="I1195" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="1196" spans="1:9">
-      <c r="A1196" t="s">
-        <v>1683</v>
-      </c>
-      <c r="C1196" t="s">
-        <v>600</v>
-      </c>
-      <c r="E1196" t="s">
-        <v>661</v>
-      </c>
-      <c r="F1196" t="s">
-        <v>1684</v>
-      </c>
-      <c r="I1196" t="s">
-        <v>1127</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1197" spans="1:9">
@@ -26993,13 +26979,13 @@
         <v>600</v>
       </c>
       <c r="E1197" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F1197" t="s">
         <v>1684</v>
       </c>
       <c r="I1197" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1198" spans="1:9">
@@ -27010,33 +26996,30 @@
         <v>600</v>
       </c>
       <c r="E1198" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F1198" t="s">
         <v>1684</v>
       </c>
       <c r="I1198" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1199" spans="1:9">
       <c r="A1199" t="s">
         <v>1683</v>
       </c>
-      <c r="B1199" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1199" t="s">
         <v>600</v>
       </c>
       <c r="E1199" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F1199" t="s">
         <v>1684</v>
       </c>
       <c r="I1199" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1200" spans="1:9">
@@ -27047,64 +27030,67 @@
         <v>600</v>
       </c>
       <c r="E1200" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F1200" t="s">
         <v>1684</v>
       </c>
       <c r="I1200" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1201" spans="1:9">
       <c r="A1201" t="s">
         <v>1683</v>
       </c>
+      <c r="B1201" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1201" t="s">
         <v>600</v>
       </c>
       <c r="E1201" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F1201" t="s">
         <v>1684</v>
       </c>
       <c r="I1201" t="s">
-        <v>1132</v>
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:9">
+      <c r="A1202" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C1202" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1202" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1202" t="s">
+        <v>1684</v>
+      </c>
+      <c r="I1202" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="1203" spans="1:9">
       <c r="A1203" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
       <c r="C1203" t="s">
         <v>600</v>
       </c>
       <c r="E1203" t="s">
-        <v>658</v>
+        <v>666</v>
       </c>
       <c r="F1203" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
       <c r="I1203" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="1204" spans="1:9">
-      <c r="A1204" t="s">
-        <v>1685</v>
-      </c>
-      <c r="C1204" t="s">
-        <v>600</v>
-      </c>
-      <c r="E1204" t="s">
-        <v>661</v>
-      </c>
-      <c r="F1204" t="s">
-        <v>1686</v>
-      </c>
-      <c r="I1204" t="s">
-        <v>1127</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1205" spans="1:9">
@@ -27115,13 +27101,13 @@
         <v>600</v>
       </c>
       <c r="E1205" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F1205" t="s">
         <v>1686</v>
       </c>
       <c r="I1205" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1206" spans="1:9">
@@ -27132,33 +27118,30 @@
         <v>600</v>
       </c>
       <c r="E1206" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F1206" t="s">
         <v>1686</v>
       </c>
       <c r="I1206" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1207" spans="1:9">
       <c r="A1207" t="s">
         <v>1685</v>
       </c>
-      <c r="B1207" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1207" t="s">
         <v>600</v>
       </c>
       <c r="E1207" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F1207" t="s">
         <v>1686</v>
       </c>
       <c r="I1207" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1208" spans="1:9">
@@ -27169,68 +27152,77 @@
         <v>600</v>
       </c>
       <c r="E1208" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F1208" t="s">
         <v>1686</v>
       </c>
       <c r="I1208" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1209" spans="1:9">
       <c r="A1209" t="s">
         <v>1685</v>
       </c>
+      <c r="B1209" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1209" t="s">
         <v>600</v>
       </c>
       <c r="E1209" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F1209" t="s">
         <v>1686</v>
       </c>
       <c r="I1209" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="1210" spans="1:9">
       <c r="A1210" t="s">
-        <v>1191</v>
+        <v>1685</v>
+      </c>
+      <c r="C1210" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1210" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1210" t="s">
+        <v>1686</v>
+      </c>
+      <c r="I1210" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="1211" spans="1:9">
       <c r="A1211" t="s">
-        <v>1687</v>
+        <v>1685</v>
       </c>
       <c r="C1211" t="s">
-        <v>659</v>
+        <v>600</v>
       </c>
       <c r="E1211" t="s">
-        <v>674</v>
+        <v>666</v>
+      </c>
+      <c r="F1211" t="s">
+        <v>1686</v>
       </c>
       <c r="I1211" t="s">
-        <v>1146</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1212" spans="1:9">
       <c r="A1212" t="s">
-        <v>1687</v>
-      </c>
-      <c r="G1212" t="s">
-        <v>672</v>
-      </c>
-      <c r="H1212" t="s">
-        <v>673</v>
-      </c>
-      <c r="I1212" t="s">
-        <v>1068</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="1213" spans="1:9">
       <c r="A1213" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="C1213" t="s">
         <v>659</v>
@@ -27239,12 +27231,12 @@
         <v>674</v>
       </c>
       <c r="I1213" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="1214" spans="1:9">
       <c r="A1214" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="G1214" t="s">
         <v>672</v>
@@ -27252,13 +27244,13 @@
       <c r="H1214" t="s">
         <v>673</v>
       </c>
-      <c r="I1214" s="1" t="s">
-        <v>1074</v>
+      <c r="I1214" t="s">
+        <v>1068</v>
       </c>
     </row>
     <row r="1215" spans="1:9">
       <c r="A1215" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C1215" t="s">
         <v>659</v>
@@ -27267,12 +27259,12 @@
         <v>674</v>
       </c>
       <c r="I1215" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="1216" spans="1:9">
       <c r="A1216" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="G1216" t="s">
         <v>672</v>
@@ -27280,13 +27272,13 @@
       <c r="H1216" t="s">
         <v>673</v>
       </c>
-      <c r="I1216" t="s">
-        <v>1105</v>
+      <c r="I1216" s="1" t="s">
+        <v>1074</v>
       </c>
     </row>
     <row r="1217" spans="1:9">
       <c r="A1217" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="C1217" t="s">
         <v>659</v>
@@ -27295,12 +27287,12 @@
         <v>674</v>
       </c>
       <c r="I1217" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1218" spans="1:9">
       <c r="A1218" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="G1218" t="s">
         <v>672</v>
@@ -27309,15 +27301,12 @@
         <v>673</v>
       </c>
       <c r="I1218" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="1219" spans="1:9">
       <c r="A1219" t="s">
-        <v>1691</v>
-      </c>
-      <c r="B1219" t="s">
-        <v>1192</v>
+        <v>1690</v>
       </c>
       <c r="C1219" t="s">
         <v>659</v>
@@ -27326,15 +27315,12 @@
         <v>674</v>
       </c>
       <c r="I1219" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="1220" spans="1:9">
       <c r="A1220" t="s">
-        <v>1691</v>
-      </c>
-      <c r="B1220" t="s">
-        <v>1192</v>
+        <v>1690</v>
       </c>
       <c r="G1220" t="s">
         <v>672</v>
@@ -27343,12 +27329,15 @@
         <v>673</v>
       </c>
       <c r="I1220" t="s">
-        <v>1833</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="1221" spans="1:9">
       <c r="A1221" t="s">
-        <v>1692</v>
+        <v>1691</v>
+      </c>
+      <c r="B1221" t="s">
+        <v>1192</v>
       </c>
       <c r="C1221" t="s">
         <v>659</v>
@@ -27357,12 +27346,15 @@
         <v>674</v>
       </c>
       <c r="I1221" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1222" spans="1:9">
       <c r="A1222" t="s">
-        <v>1692</v>
+        <v>1691</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>1192</v>
       </c>
       <c r="G1222" t="s">
         <v>672</v>
@@ -27371,12 +27363,12 @@
         <v>673</v>
       </c>
       <c r="I1222" t="s">
-        <v>1108</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="1223" spans="1:9">
       <c r="A1223" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="C1223" t="s">
         <v>659</v>
@@ -27385,12 +27377,12 @@
         <v>674</v>
       </c>
       <c r="I1223" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1224" spans="1:9">
       <c r="A1224" t="s">
-        <v>1789</v>
+        <v>1692</v>
       </c>
       <c r="G1224" t="s">
         <v>672</v>
@@ -27398,38 +27390,38 @@
       <c r="H1224" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="1227" spans="1:9">
-      <c r="A1227" t="s">
-        <v>1694</v>
-      </c>
-      <c r="C1227" t="s">
-        <v>585</v>
-      </c>
-      <c r="E1227" t="s">
+      <c r="I1224" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:9">
+      <c r="A1225" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C1225" t="s">
+        <v>659</v>
+      </c>
+      <c r="E1225" t="s">
         <v>674</v>
       </c>
-      <c r="I1227" t="s">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="1228" spans="1:9">
-      <c r="A1228" t="s">
-        <v>1694</v>
-      </c>
-      <c r="G1228" t="s">
+      <c r="I1225" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:9">
+      <c r="A1226" t="s">
+        <v>1789</v>
+      </c>
+      <c r="G1226" t="s">
         <v>672</v>
       </c>
-      <c r="H1228" t="s">
+      <c r="H1226" t="s">
         <v>673</v>
-      </c>
-      <c r="I1228" t="s">
-        <v>1068</v>
       </c>
     </row>
     <row r="1229" spans="1:9">
       <c r="A1229" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="C1229" t="s">
         <v>585</v>
@@ -27438,12 +27430,12 @@
         <v>674</v>
       </c>
       <c r="I1229" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="1230" spans="1:9">
       <c r="A1230" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="G1230" t="s">
         <v>672</v>
@@ -27451,13 +27443,13 @@
       <c r="H1230" t="s">
         <v>673</v>
       </c>
-      <c r="I1230" s="1" t="s">
-        <v>1074</v>
+      <c r="I1230" t="s">
+        <v>1068</v>
       </c>
     </row>
     <row r="1231" spans="1:9">
       <c r="A1231" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="C1231" t="s">
         <v>585</v>
@@ -27466,12 +27458,12 @@
         <v>674</v>
       </c>
       <c r="I1231" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="1232" spans="1:9">
       <c r="A1232" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="G1232" t="s">
         <v>672</v>
@@ -27479,13 +27471,13 @@
       <c r="H1232" t="s">
         <v>673</v>
       </c>
-      <c r="I1232" t="s">
-        <v>1105</v>
+      <c r="I1232" s="1" t="s">
+        <v>1074</v>
       </c>
     </row>
     <row r="1233" spans="1:9">
       <c r="A1233" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="C1233" t="s">
         <v>585</v>
@@ -27494,12 +27486,12 @@
         <v>674</v>
       </c>
       <c r="I1233" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1234" spans="1:9">
       <c r="A1234" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="G1234" t="s">
         <v>672</v>
@@ -27508,15 +27500,12 @@
         <v>673</v>
       </c>
       <c r="I1234" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="1235" spans="1:9">
       <c r="A1235" t="s">
-        <v>1698</v>
-      </c>
-      <c r="B1235" t="s">
-        <v>1192</v>
+        <v>1697</v>
       </c>
       <c r="C1235" t="s">
         <v>585</v>
@@ -27525,15 +27514,12 @@
         <v>674</v>
       </c>
       <c r="I1235" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="1236" spans="1:9">
       <c r="A1236" t="s">
-        <v>1698</v>
-      </c>
-      <c r="B1236" t="s">
-        <v>1192</v>
+        <v>1697</v>
       </c>
       <c r="G1236" t="s">
         <v>672</v>
@@ -27542,12 +27528,15 @@
         <v>673</v>
       </c>
       <c r="I1236" t="s">
-        <v>1833</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="1237" spans="1:9">
       <c r="A1237" t="s">
-        <v>1699</v>
+        <v>1698</v>
+      </c>
+      <c r="B1237" t="s">
+        <v>1192</v>
       </c>
       <c r="C1237" t="s">
         <v>585</v>
@@ -27556,12 +27545,15 @@
         <v>674</v>
       </c>
       <c r="I1237" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1238" spans="1:9">
       <c r="A1238" t="s">
-        <v>1699</v>
+        <v>1698</v>
+      </c>
+      <c r="B1238" t="s">
+        <v>1192</v>
       </c>
       <c r="G1238" t="s">
         <v>672</v>
@@ -27570,12 +27562,12 @@
         <v>673</v>
       </c>
       <c r="I1238" t="s">
-        <v>1108</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="1239" spans="1:9">
       <c r="A1239" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="C1239" t="s">
         <v>585</v>
@@ -27584,12 +27576,12 @@
         <v>674</v>
       </c>
       <c r="I1239" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1240" spans="1:9">
       <c r="A1240" t="s">
-        <v>1788</v>
+        <v>1699</v>
       </c>
       <c r="G1240" t="s">
         <v>672</v>
@@ -27597,173 +27589,173 @@
       <c r="H1240" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="1243" spans="1:9">
-      <c r="A1243" t="s">
-        <v>1701</v>
-      </c>
-      <c r="C1243" t="s">
-        <v>659</v>
-      </c>
-      <c r="E1243" t="s">
+      <c r="I1240" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:9">
+      <c r="A1241" t="s">
+        <v>1700</v>
+      </c>
+      <c r="C1241" t="s">
+        <v>585</v>
+      </c>
+      <c r="E1241" t="s">
         <v>674</v>
       </c>
-      <c r="I1243" t="s">
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="1244" spans="1:9">
-      <c r="A1244" t="s">
-        <v>1702</v>
-      </c>
-      <c r="C1244" t="s">
-        <v>659</v>
-      </c>
-      <c r="E1244" t="s">
-        <v>674</v>
-      </c>
-      <c r="I1244" t="s">
-        <v>1147</v>
+      <c r="I1241" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:9">
+      <c r="A1242" t="s">
+        <v>1788</v>
+      </c>
+      <c r="G1242" t="s">
+        <v>672</v>
+      </c>
+      <c r="H1242" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="1245" spans="1:9">
       <c r="A1245" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C1245" t="s">
+        <v>659</v>
+      </c>
+      <c r="E1245" t="s">
+        <v>674</v>
+      </c>
+      <c r="I1245" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:9">
+      <c r="A1246" t="s">
         <v>1702</v>
       </c>
-      <c r="G1245" t="s">
-        <v>672</v>
-      </c>
-      <c r="H1245" t="s">
-        <v>673</v>
-      </c>
-      <c r="I1245" s="1" t="s">
-        <v>1074</v>
+      <c r="C1246" t="s">
+        <v>659</v>
+      </c>
+      <c r="E1246" t="s">
+        <v>674</v>
+      </c>
+      <c r="I1246" t="s">
+        <v>1147</v>
       </c>
     </row>
     <row r="1247" spans="1:9">
       <c r="A1247" t="s">
-        <v>1703</v>
-      </c>
-      <c r="C1247" t="s">
-        <v>659</v>
-      </c>
-      <c r="E1247" t="s">
-        <v>674</v>
-      </c>
-      <c r="I1247" t="s">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="1248" spans="1:9">
-      <c r="A1248" t="s">
-        <v>1704</v>
-      </c>
-      <c r="C1248" t="s">
-        <v>659</v>
-      </c>
-      <c r="E1248" t="s">
-        <v>674</v>
-      </c>
-      <c r="I1248" t="s">
-        <v>1148</v>
+        <v>1702</v>
+      </c>
+      <c r="G1247" t="s">
+        <v>672</v>
+      </c>
+      <c r="H1247" t="s">
+        <v>673</v>
+      </c>
+      <c r="I1247" s="1" t="s">
+        <v>1074</v>
       </c>
     </row>
     <row r="1249" spans="1:9">
       <c r="A1249" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C1249" t="s">
+        <v>659</v>
+      </c>
+      <c r="E1249" t="s">
+        <v>674</v>
+      </c>
+      <c r="I1249" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:9">
+      <c r="A1250" t="s">
         <v>1704</v>
       </c>
-      <c r="G1249" t="s">
-        <v>672</v>
-      </c>
-      <c r="H1249" t="s">
-        <v>673</v>
-      </c>
-      <c r="I1249" t="s">
-        <v>1105</v>
+      <c r="C1250" t="s">
+        <v>659</v>
+      </c>
+      <c r="E1250" t="s">
+        <v>674</v>
+      </c>
+      <c r="I1250" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="1251" spans="1:9">
       <c r="A1251" t="s">
-        <v>1705</v>
-      </c>
-      <c r="B1251" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C1251" t="s">
-        <v>659</v>
-      </c>
-      <c r="E1251" t="s">
-        <v>674</v>
+        <v>1704</v>
+      </c>
+      <c r="G1251" t="s">
+        <v>672</v>
+      </c>
+      <c r="H1251" t="s">
+        <v>673</v>
       </c>
       <c r="I1251" t="s">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="1252" spans="1:9">
-      <c r="A1252" t="s">
-        <v>1706</v>
-      </c>
-      <c r="B1252" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C1252" t="s">
-        <v>659</v>
-      </c>
-      <c r="E1252" t="s">
-        <v>674</v>
-      </c>
-      <c r="I1252" t="s">
-        <v>1150</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="1253" spans="1:9">
       <c r="A1253" t="s">
+        <v>1705</v>
+      </c>
+      <c r="B1253" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C1253" t="s">
+        <v>659</v>
+      </c>
+      <c r="E1253" t="s">
+        <v>674</v>
+      </c>
+      <c r="I1253" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:9">
+      <c r="A1254" t="s">
         <v>1706</v>
       </c>
-      <c r="B1253" t="s">
-        <v>1192</v>
-      </c>
-      <c r="G1253" t="s">
-        <v>672</v>
-      </c>
-      <c r="H1253" t="s">
-        <v>673</v>
-      </c>
-      <c r="I1253" t="s">
-        <v>1833</v>
+      <c r="B1254" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C1254" t="s">
+        <v>659</v>
+      </c>
+      <c r="E1254" t="s">
+        <v>674</v>
+      </c>
+      <c r="I1254" t="s">
+        <v>1150</v>
       </c>
     </row>
     <row r="1255" spans="1:9">
       <c r="A1255" t="s">
-        <v>1707</v>
-      </c>
-      <c r="C1255" t="s">
-        <v>659</v>
-      </c>
-      <c r="E1255" t="s">
-        <v>674</v>
+        <v>1706</v>
+      </c>
+      <c r="B1255" t="s">
+        <v>1192</v>
+      </c>
+      <c r="G1255" t="s">
+        <v>672</v>
+      </c>
+      <c r="H1255" t="s">
+        <v>673</v>
       </c>
       <c r="I1255" t="s">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="1256" spans="1:9">
-      <c r="A1256" t="s">
-        <v>1707</v>
-      </c>
-      <c r="G1256" t="s">
-        <v>672</v>
-      </c>
-      <c r="H1256" t="s">
-        <v>673</v>
-      </c>
-      <c r="I1256" t="s">
-        <v>1068</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="1257" spans="1:9">
       <c r="A1257" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="C1257" t="s">
         <v>659</v>
@@ -27772,12 +27764,12 @@
         <v>674</v>
       </c>
       <c r="I1257" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="1258" spans="1:9">
       <c r="A1258" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="G1258" t="s">
         <v>672</v>
@@ -27785,13 +27777,13 @@
       <c r="H1258" t="s">
         <v>673</v>
       </c>
-      <c r="I1258" s="1" t="s">
-        <v>1074</v>
+      <c r="I1258" t="s">
+        <v>1068</v>
       </c>
     </row>
     <row r="1259" spans="1:9">
       <c r="A1259" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="C1259" t="s">
         <v>659</v>
@@ -27800,12 +27792,12 @@
         <v>674</v>
       </c>
       <c r="I1259" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="1260" spans="1:9">
       <c r="A1260" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="G1260" t="s">
         <v>672</v>
@@ -27813,13 +27805,13 @@
       <c r="H1260" t="s">
         <v>673</v>
       </c>
-      <c r="I1260" t="s">
-        <v>1105</v>
+      <c r="I1260" s="1" t="s">
+        <v>1074</v>
       </c>
     </row>
     <row r="1261" spans="1:9">
       <c r="A1261" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="C1261" t="s">
         <v>659</v>
@@ -27828,12 +27820,12 @@
         <v>674</v>
       </c>
       <c r="I1261" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1262" spans="1:9">
       <c r="A1262" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="G1262" t="s">
         <v>672</v>
@@ -27842,15 +27834,12 @@
         <v>673</v>
       </c>
       <c r="I1262" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="1263" spans="1:9">
       <c r="A1263" t="s">
-        <v>1711</v>
-      </c>
-      <c r="B1263" t="s">
-        <v>1192</v>
+        <v>1710</v>
       </c>
       <c r="C1263" t="s">
         <v>659</v>
@@ -27859,15 +27848,12 @@
         <v>674</v>
       </c>
       <c r="I1263" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="1264" spans="1:9">
       <c r="A1264" t="s">
-        <v>1711</v>
-      </c>
-      <c r="B1264" t="s">
-        <v>1192</v>
+        <v>1710</v>
       </c>
       <c r="G1264" t="s">
         <v>672</v>
@@ -27876,12 +27862,15 @@
         <v>673</v>
       </c>
       <c r="I1264" t="s">
-        <v>1833</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="1265" spans="1:9">
       <c r="A1265" t="s">
-        <v>1712</v>
+        <v>1711</v>
+      </c>
+      <c r="B1265" t="s">
+        <v>1192</v>
       </c>
       <c r="C1265" t="s">
         <v>659</v>
@@ -27890,12 +27879,15 @@
         <v>674</v>
       </c>
       <c r="I1265" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1266" spans="1:9">
       <c r="A1266" t="s">
-        <v>1712</v>
+        <v>1711</v>
+      </c>
+      <c r="B1266" t="s">
+        <v>1192</v>
       </c>
       <c r="G1266" t="s">
         <v>672</v>
@@ -27904,12 +27896,12 @@
         <v>673</v>
       </c>
       <c r="I1266" t="s">
-        <v>1108</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="1267" spans="1:9">
       <c r="A1267" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="C1267" t="s">
         <v>659</v>
@@ -27918,12 +27910,12 @@
         <v>674</v>
       </c>
       <c r="I1267" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1268" spans="1:9">
       <c r="A1268" t="s">
-        <v>1790</v>
+        <v>1712</v>
       </c>
       <c r="G1268" t="s">
         <v>672</v>
@@ -27931,39 +27923,33 @@
       <c r="H1268" t="s">
         <v>673</v>
       </c>
+      <c r="I1268" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:9">
+      <c r="A1269" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C1269" t="s">
+        <v>659</v>
+      </c>
+      <c r="E1269" t="s">
+        <v>674</v>
+      </c>
+      <c r="I1269" t="s">
+        <v>1152</v>
+      </c>
     </row>
     <row r="1270" spans="1:9">
       <c r="A1270" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C1270" t="s">
-        <v>600</v>
-      </c>
-      <c r="E1270" t="s">
-        <v>658</v>
-      </c>
-      <c r="F1270" t="s">
-        <v>1715</v>
-      </c>
-      <c r="I1270" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="1271" spans="1:9">
-      <c r="A1271" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C1271" t="s">
-        <v>600</v>
-      </c>
-      <c r="E1271" t="s">
-        <v>661</v>
-      </c>
-      <c r="F1271" t="s">
-        <v>1715</v>
-      </c>
-      <c r="I1271" t="s">
-        <v>1127</v>
+        <v>1790</v>
+      </c>
+      <c r="G1270" t="s">
+        <v>672</v>
+      </c>
+      <c r="H1270" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="1272" spans="1:9">
@@ -27974,13 +27960,13 @@
         <v>600</v>
       </c>
       <c r="E1272" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F1272" t="s">
         <v>1715</v>
       </c>
       <c r="I1272" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="1273" spans="1:9">
@@ -27991,33 +27977,30 @@
         <v>600</v>
       </c>
       <c r="E1273" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F1273" t="s">
         <v>1715</v>
       </c>
       <c r="I1273" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1274" spans="1:9">
       <c r="A1274" t="s">
         <v>1714</v>
       </c>
-      <c r="B1274" t="s">
-        <v>1192</v>
-      </c>
       <c r="C1274" t="s">
         <v>600</v>
       </c>
       <c r="E1274" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F1274" t="s">
         <v>1715</v>
       </c>
       <c r="I1274" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="1275" spans="1:9">
@@ -28028,29 +28011,66 @@
         <v>600</v>
       </c>
       <c r="E1275" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F1275" t="s">
         <v>1715</v>
       </c>
       <c r="I1275" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="1276" spans="1:9">
       <c r="A1276" t="s">
         <v>1714</v>
       </c>
+      <c r="B1276" t="s">
+        <v>1192</v>
+      </c>
       <c r="C1276" t="s">
         <v>600</v>
       </c>
       <c r="E1276" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F1276" t="s">
         <v>1715</v>
       </c>
       <c r="I1276" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:9">
+      <c r="A1277" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C1277" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1277" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1277" t="s">
+        <v>1715</v>
+      </c>
+      <c r="I1277" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:9">
+      <c r="A1278" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C1278" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1278" t="s">
+        <v>666</v>
+      </c>
+      <c r="F1278" t="s">
+        <v>1715</v>
+      </c>
+      <c r="I1278" t="s">
         <v>1132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mass mail method permissions for signup role
</commit_message>
<xml_diff>
--- a/permission_definitions.xlsx
+++ b/permission_definitions.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8191" uniqueCount="1978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8191" uniqueCount="1980">
   <si>
     <t>INVENTORY_DB</t>
   </si>
@@ -5960,6 +5960,12 @@
   </si>
   <si>
     <t>org.phoenixctms.ctsms.service.massmail.MassMailService.getMassMailCount</t>
+  </si>
+  <si>
+    <t>MASS_MAIL_MASTER_ALL_DEPARTMENTS:MASS_MAIL_DETAIL_ALL_DEPARTMENTS:MASS_MAIL_VIEW_ALL_DEPARTMENTS:MASS_MAIL_SIGNUP, MASS_MAIL_MASTER_USER_DEPARTMENT:MASS_MAIL_DETAIL_USER_DEPARTMENT:MASS_MAIL_VIEW_USER_DEPARTMENT</t>
+  </si>
+  <si>
+    <t>PROBAND_MASTER_ALL_DEPARTMENTS:PROBAND_DETAIL_ALL_DEPARTMENTS:MASS_MAIL_SIGNUP, PROBAND_MASTER_USER_DEPARTMENT:PROBAND_DETAIL_USER_DEPARTMENT</t>
   </si>
 </sst>
 </file>
@@ -9033,8 +9039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I1400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A802" workbookViewId="0">
-      <selection activeCell="A839" sqref="A839"/>
+    <sheetView tabSelected="1" topLeftCell="A786" workbookViewId="0">
+      <selection activeCell="A819" sqref="A819"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -20828,7 +20834,7 @@
         <v>1939</v>
       </c>
       <c r="I796" t="s">
-        <v>1915</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="798" spans="1:9">
@@ -21140,7 +21146,7 @@
         <v>1939</v>
       </c>
       <c r="I818" t="s">
-        <v>1912</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="819" spans="1:9">
@@ -21160,7 +21166,7 @@
         <v>72</v>
       </c>
       <c r="I819" t="s">
-        <v>1106</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="820" spans="1:9">

</xml_diff>

<commit_message>
fix user settings page method permissions
</commit_message>
<xml_diff>
--- a/permission_definitions.xlsx
+++ b/permission_definitions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5083" uniqueCount="1409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5083" uniqueCount="1410">
   <si>
     <t>#SERVICE_METHOD</t>
   </si>
@@ -4241,6 +4241,9 @@
   </si>
   <si>
     <t>ANY_USER</t>
+  </si>
+  <si>
+    <t>org.phoenixctms.ctsms.service.user.UserService.updateUserSettings</t>
   </si>
 </sst>
 </file>
@@ -5068,7 +5071,7 @@
   <dimension ref="A1:I1016"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A637" workbookViewId="0">
-      <selection activeCell="A656" sqref="A656"/>
+      <selection activeCell="A671" sqref="A671"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -16227,7 +16230,7 @@
     </row>
     <row r="671" spans="1:9" s="2" customFormat="1">
       <c r="A671" s="2" t="s">
-        <v>986</v>
+        <v>1409</v>
       </c>
       <c r="C671" s="2" t="s">
         <v>1406</v>

</xml_diff>